<commit_message>
renombramiento de variables del share_data y ya funciona las variables de sesion
</commit_message>
<xml_diff>
--- a/public/recursos/Cotizacion-modulos.xlsx
+++ b/public/recursos/Cotizacion-modulos.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WWW\avaluamos\public\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9DA1E0E-C556-4ED2-9F88-74500BBE426F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C1B0BF-C92F-4E3D-83FF-AFA151831BB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diseño" sheetId="1" r:id="rId1"/>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="265">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="266">
   <si>
     <t>HEADER</t>
   </si>
@@ -844,6 +844,9 @@
     <t>1. Incluye soporte por 4 meses
 2. El tiempo adicional es asumido por el desarrollador
 3. Las solicitudes adicionales serán negociadas y asumidas con valor adicional</t>
+  </si>
+  <si>
+    <t>Informe Avalúo (Cálculos)</t>
   </si>
 </sst>
 </file>
@@ -1248,7 +1251,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="101">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1391,6 +1394,30 @@
     <xf numFmtId="164" fontId="1" fillId="5" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1478,74 +1505,53 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1846,13 +1852,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="53" t="s">
+      <c r="A1" s="61" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="53"/>
-      <c r="C1" s="53"/>
-      <c r="D1" s="53"/>
-      <c r="E1" s="53"/>
+      <c r="B1" s="61"/>
+      <c r="C1" s="61"/>
+      <c r="D1" s="61"/>
+      <c r="E1" s="61"/>
     </row>
     <row r="2" spans="1:9" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="41"/>
@@ -1882,20 +1888,20 @@
       <c r="E3" s="42"/>
     </row>
     <row r="4" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="54" t="s">
+      <c r="A4" s="62" t="s">
         <v>234</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>243</v>
       </c>
-      <c r="C4" s="55">
+      <c r="C4" s="63">
         <v>2</v>
       </c>
-      <c r="D4" s="68">
+      <c r="D4" s="76">
         <f>H9*5%</f>
         <v>510000</v>
       </c>
-      <c r="E4" s="58" t="s">
+      <c r="E4" s="66" t="s">
         <v>250</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -1906,13 +1912,13 @@
       </c>
     </row>
     <row r="5" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="55"/>
+      <c r="A5" s="63"/>
       <c r="B5" s="29" t="s">
         <v>235</v>
       </c>
-      <c r="C5" s="55"/>
-      <c r="D5" s="55"/>
-      <c r="E5" s="59"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="67"/>
       <c r="G5" s="1" t="s">
         <v>246</v>
       </c>
@@ -1925,7 +1931,7 @@
       <c r="B6" s="31"/>
       <c r="C6" s="35"/>
       <c r="D6" s="35"/>
-      <c r="E6" s="59"/>
+      <c r="E6" s="67"/>
       <c r="G6" s="1" t="s">
         <v>246</v>
       </c>
@@ -1935,10 +1941,10 @@
       </c>
     </row>
     <row r="7" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="62" t="s">
+      <c r="A7" s="70" t="s">
         <v>236</v>
       </c>
-      <c r="B7" s="63"/>
+      <c r="B7" s="71"/>
       <c r="C7" s="36">
         <v>2</v>
       </c>
@@ -1946,7 +1952,7 @@
         <f>H9*10%</f>
         <v>1020000</v>
       </c>
-      <c r="E7" s="59"/>
+      <c r="E7" s="67"/>
       <c r="G7" s="1" t="s">
         <v>247</v>
       </c>
@@ -1959,10 +1965,10 @@
       </c>
     </row>
     <row r="8" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="60" t="s">
+      <c r="A8" s="68" t="s">
         <v>232</v>
       </c>
-      <c r="B8" s="61"/>
+      <c r="B8" s="69"/>
       <c r="C8" s="37">
         <v>1</v>
       </c>
@@ -1970,10 +1976,10 @@
         <f>H9*10%</f>
         <v>1020000</v>
       </c>
-      <c r="E8" s="59"/>
+      <c r="E8" s="67"/>
     </row>
     <row r="9" spans="1:9" ht="30" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="56" t="s">
+      <c r="A9" s="64" t="s">
         <v>1</v>
       </c>
       <c r="B9" s="3" t="s">
@@ -1982,29 +1988,29 @@
       <c r="C9" s="38">
         <v>1</v>
       </c>
-      <c r="D9" s="69">
+      <c r="D9" s="77">
         <f>H9*60%</f>
         <v>6120000</v>
       </c>
-      <c r="E9" s="59"/>
+      <c r="E9" s="67"/>
       <c r="H9" s="43">
         <f>C3*H6</f>
         <v>10200000</v>
       </c>
     </row>
     <row r="10" spans="1:9" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="57"/>
+      <c r="A10" s="65"/>
       <c r="B10" s="4" t="s">
         <v>231</v>
       </c>
       <c r="C10" s="38">
         <v>3</v>
       </c>
-      <c r="D10" s="70"/>
-      <c r="E10" s="59"/>
+      <c r="D10" s="78"/>
+      <c r="E10" s="67"/>
     </row>
     <row r="11" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="64" t="s">
+      <c r="A11" s="72" t="s">
         <v>238</v>
       </c>
       <c r="B11" s="34" t="s">
@@ -2017,14 +2023,14 @@
         <f>H9*7.5%</f>
         <v>765000</v>
       </c>
-      <c r="E11" s="59"/>
+      <c r="E11" s="67"/>
       <c r="H11" s="43">
         <f>H7*5</f>
         <v>17000000</v>
       </c>
     </row>
     <row r="12" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="65"/>
+      <c r="A12" s="73"/>
       <c r="B12" s="34" t="s">
         <v>240</v>
       </c>
@@ -2035,14 +2041,14 @@
         <f>H9*7.5%</f>
         <v>765000</v>
       </c>
-      <c r="E12" s="59"/>
+      <c r="E12" s="67"/>
     </row>
     <row r="13" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="30"/>
       <c r="B13" s="31"/>
       <c r="C13" s="35"/>
       <c r="D13" s="35"/>
-      <c r="E13" s="59"/>
+      <c r="E13" s="67"/>
     </row>
     <row r="14" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="30"/>
@@ -2052,28 +2058,28 @@
         <f>SUM(D4:D12)</f>
         <v>10200000</v>
       </c>
-      <c r="E14" s="59"/>
+      <c r="E14" s="67"/>
     </row>
     <row r="15" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="74" t="s">
         <v>241</v>
       </c>
-      <c r="B15" s="67"/>
+      <c r="B15" s="75"/>
       <c r="C15" s="39"/>
       <c r="D15" s="39"/>
-      <c r="E15" s="59"/>
+      <c r="E15" s="67"/>
     </row>
     <row r="16" spans="1:9" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="51" t="s">
+      <c r="A16" s="59" t="s">
         <v>237</v>
       </c>
-      <c r="B16" s="52"/>
+      <c r="B16" s="60"/>
       <c r="C16" s="35"/>
       <c r="D16" s="46">
         <f>D14*10%</f>
         <v>1020000</v>
       </c>
-      <c r="E16" s="59"/>
+      <c r="E16" s="67"/>
     </row>
     <row r="17" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="32" t="s">
@@ -2085,25 +2091,25 @@
         <f>D14-D16</f>
         <v>9180000</v>
       </c>
-      <c r="E17" s="59"/>
+      <c r="E17" s="67"/>
     </row>
     <row r="18" spans="1:5" ht="30" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="51" t="s">
+      <c r="A18" s="59" t="s">
         <v>3</v>
       </c>
-      <c r="B18" s="52"/>
+      <c r="B18" s="60"/>
       <c r="C18" s="35"/>
       <c r="D18" s="35"/>
-      <c r="E18" s="59"/>
+      <c r="E18" s="67"/>
     </row>
     <row r="19" spans="1:5" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="48" t="s">
+      <c r="A19" s="56" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="49"/>
-      <c r="C19" s="49"/>
-      <c r="D19" s="49"/>
-      <c r="E19" s="50"/>
+      <c r="B19" s="57"/>
+      <c r="C19" s="57"/>
+      <c r="D19" s="57"/>
+      <c r="E19" s="58"/>
     </row>
     <row r="20" spans="1:5" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3"/>
   </sheetData>
@@ -2147,12 +2153,12 @@
   <sheetData>
     <row r="1" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="72" t="s">
+      <c r="A2" s="80" t="s">
         <v>17</v>
       </c>
-      <c r="B2" s="72"/>
-      <c r="C2" s="72"/>
-      <c r="D2" s="72"/>
+      <c r="B2" s="80"/>
+      <c r="C2" s="80"/>
+      <c r="D2" s="80"/>
     </row>
     <row r="3" spans="1:4" ht="16.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
@@ -2169,7 +2175,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="76" t="s">
+      <c r="A4" s="84" t="s">
         <v>16</v>
       </c>
       <c r="B4" s="8" t="s">
@@ -2179,7 +2185,7 @@
       <c r="D4" s="20"/>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="71"/>
+      <c r="A5" s="79"/>
       <c r="B5" s="10" t="s">
         <v>6</v>
       </c>
@@ -2187,7 +2193,7 @@
       <c r="D5" s="21"/>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="71"/>
+      <c r="A6" s="79"/>
       <c r="B6" s="10" t="s">
         <v>7</v>
       </c>
@@ -2195,7 +2201,7 @@
       <c r="D6" s="21"/>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="71"/>
+      <c r="A7" s="79"/>
       <c r="B7" s="10" t="s">
         <v>8</v>
       </c>
@@ -2203,7 +2209,7 @@
       <c r="D7" s="21"/>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="71"/>
+      <c r="A8" s="79"/>
       <c r="B8" s="10" t="s">
         <v>9</v>
       </c>
@@ -2227,7 +2233,7 @@
       <c r="D10" s="21"/>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="71" t="s">
+      <c r="A11" s="79" t="s">
         <v>14</v>
       </c>
       <c r="B11" s="10" t="s">
@@ -2237,7 +2243,7 @@
       <c r="D11" s="21"/>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="71"/>
+      <c r="A12" s="79"/>
       <c r="B12" s="10" t="s">
         <v>13</v>
       </c>
@@ -2245,7 +2251,7 @@
       <c r="D12" s="21"/>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="71"/>
+      <c r="A13" s="79"/>
       <c r="B13" s="10" t="s">
         <v>18</v>
       </c>
@@ -2253,7 +2259,7 @@
       <c r="D13" s="21"/>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="71" t="s">
+      <c r="A14" s="79" t="s">
         <v>19</v>
       </c>
       <c r="B14" s="10" t="s">
@@ -2263,7 +2269,7 @@
       <c r="D14" s="21"/>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="71"/>
+      <c r="A15" s="79"/>
       <c r="B15" s="10" t="s">
         <v>21</v>
       </c>
@@ -2271,7 +2277,7 @@
       <c r="D15" s="21"/>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="71"/>
+      <c r="A16" s="79"/>
       <c r="B16" s="10" t="s">
         <v>22</v>
       </c>
@@ -2279,7 +2285,7 @@
       <c r="D16" s="21"/>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="71" t="s">
+      <c r="A17" s="79" t="s">
         <v>23</v>
       </c>
       <c r="B17" s="10" t="s">
@@ -2289,7 +2295,7 @@
       <c r="D17" s="21"/>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="71"/>
+      <c r="A18" s="79"/>
       <c r="B18" s="10" t="s">
         <v>25</v>
       </c>
@@ -2297,7 +2303,7 @@
       <c r="D18" s="21"/>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="71" t="s">
+      <c r="A19" s="79" t="s">
         <v>26</v>
       </c>
       <c r="B19" s="10" t="s">
@@ -2307,7 +2313,7 @@
       <c r="D19" s="21"/>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="71"/>
+      <c r="A20" s="79"/>
       <c r="B20" s="10" t="s">
         <v>28</v>
       </c>
@@ -2315,7 +2321,7 @@
       <c r="D20" s="21"/>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="71"/>
+      <c r="A21" s="79"/>
       <c r="B21" s="10" t="s">
         <v>29</v>
       </c>
@@ -2323,7 +2329,7 @@
       <c r="D21" s="21"/>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="71"/>
+      <c r="A22" s="79"/>
       <c r="B22" s="10" t="s">
         <v>30</v>
       </c>
@@ -2331,7 +2337,7 @@
       <c r="D22" s="21"/>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="71"/>
+      <c r="A23" s="79"/>
       <c r="B23" s="10" t="s">
         <v>32</v>
       </c>
@@ -2339,7 +2345,7 @@
       <c r="D23" s="21"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="71"/>
+      <c r="A24" s="79"/>
       <c r="B24" s="10" t="s">
         <v>31</v>
       </c>
@@ -2347,7 +2353,7 @@
       <c r="D24" s="21"/>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="71" t="s">
+      <c r="A25" s="79" t="s">
         <v>33</v>
       </c>
       <c r="B25" s="10" t="s">
@@ -2357,7 +2363,7 @@
       <c r="D25" s="21"/>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="71"/>
+      <c r="A26" s="79"/>
       <c r="B26" s="10" t="s">
         <v>35</v>
       </c>
@@ -2365,7 +2371,7 @@
       <c r="D26" s="21"/>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="71"/>
+      <c r="A27" s="79"/>
       <c r="B27" s="10" t="s">
         <v>36</v>
       </c>
@@ -2373,7 +2379,7 @@
       <c r="D27" s="21"/>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="71"/>
+      <c r="A28" s="79"/>
       <c r="B28" s="10" t="s">
         <v>37</v>
       </c>
@@ -2381,7 +2387,7 @@
       <c r="D28" s="21"/>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="71"/>
+      <c r="A29" s="79"/>
       <c r="B29" s="10" t="s">
         <v>39</v>
       </c>
@@ -2389,7 +2395,7 @@
       <c r="D29" s="21"/>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="71"/>
+      <c r="A30" s="79"/>
       <c r="B30" s="10" t="s">
         <v>38</v>
       </c>
@@ -2397,7 +2403,7 @@
       <c r="D30" s="21"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="71"/>
+      <c r="A31" s="79"/>
       <c r="B31" s="10" t="s">
         <v>40</v>
       </c>
@@ -2405,7 +2411,7 @@
       <c r="D31" s="21"/>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A32" s="71"/>
+      <c r="A32" s="79"/>
       <c r="B32" s="10" t="s">
         <v>41</v>
       </c>
@@ -2413,7 +2419,7 @@
       <c r="D32" s="21"/>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A33" s="71"/>
+      <c r="A33" s="79"/>
       <c r="B33" s="10" t="s">
         <v>42</v>
       </c>
@@ -2421,7 +2427,7 @@
       <c r="D33" s="21"/>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A34" s="71"/>
+      <c r="A34" s="79"/>
       <c r="B34" s="10" t="s">
         <v>43</v>
       </c>
@@ -2429,7 +2435,7 @@
       <c r="D34" s="21"/>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="71"/>
+      <c r="A35" s="79"/>
       <c r="B35" s="10" t="s">
         <v>44</v>
       </c>
@@ -2437,7 +2443,7 @@
       <c r="D35" s="21"/>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" s="71"/>
+      <c r="A36" s="79"/>
       <c r="B36" s="10" t="s">
         <v>45</v>
       </c>
@@ -2445,7 +2451,7 @@
       <c r="D36" s="21"/>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="71"/>
+      <c r="A37" s="79"/>
       <c r="B37" s="10" t="s">
         <v>46</v>
       </c>
@@ -2453,7 +2459,7 @@
       <c r="D37" s="21"/>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="71"/>
+      <c r="A38" s="79"/>
       <c r="B38" s="10" t="s">
         <v>47</v>
       </c>
@@ -2461,7 +2467,7 @@
       <c r="D38" s="21"/>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="71"/>
+      <c r="A39" s="79"/>
       <c r="B39" s="10" t="s">
         <v>48</v>
       </c>
@@ -2469,7 +2475,7 @@
       <c r="D39" s="21"/>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A40" s="71"/>
+      <c r="A40" s="79"/>
       <c r="B40" s="10" t="s">
         <v>49</v>
       </c>
@@ -2487,7 +2493,7 @@
       <c r="D41" s="22"/>
     </row>
     <row r="42" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="73" t="s">
+      <c r="A42" s="81" t="s">
         <v>52</v>
       </c>
       <c r="B42" s="8" t="s">
@@ -2497,7 +2503,7 @@
       <c r="D42" s="20"/>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" s="74"/>
+      <c r="A43" s="82"/>
       <c r="B43" s="10" t="s">
         <v>54</v>
       </c>
@@ -2505,7 +2511,7 @@
       <c r="D43" s="21"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="74"/>
+      <c r="A44" s="82"/>
       <c r="B44" s="10" t="s">
         <v>55</v>
       </c>
@@ -2513,7 +2519,7 @@
       <c r="D44" s="21"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="74"/>
+      <c r="A45" s="82"/>
       <c r="B45" s="10" t="s">
         <v>56</v>
       </c>
@@ -2521,7 +2527,7 @@
       <c r="D45" s="21"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="74"/>
+      <c r="A46" s="82"/>
       <c r="B46" s="10" t="s">
         <v>57</v>
       </c>
@@ -2529,7 +2535,7 @@
       <c r="D46" s="21"/>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A47" s="74"/>
+      <c r="A47" s="82"/>
       <c r="B47" s="10" t="s">
         <v>58</v>
       </c>
@@ -2537,7 +2543,7 @@
       <c r="D47" s="21"/>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A48" s="74"/>
+      <c r="A48" s="82"/>
       <c r="B48" s="10" t="s">
         <v>59</v>
       </c>
@@ -2545,7 +2551,7 @@
       <c r="D48" s="21"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="74"/>
+      <c r="A49" s="82"/>
       <c r="B49" s="10" t="s">
         <v>60</v>
       </c>
@@ -2553,7 +2559,7 @@
       <c r="D49" s="21"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="74"/>
+      <c r="A50" s="82"/>
       <c r="B50" s="10" t="s">
         <v>61</v>
       </c>
@@ -2561,7 +2567,7 @@
       <c r="D50" s="21"/>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A51" s="74"/>
+      <c r="A51" s="82"/>
       <c r="B51" s="10" t="s">
         <v>62</v>
       </c>
@@ -2569,7 +2575,7 @@
       <c r="D51" s="21"/>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A52" s="74"/>
+      <c r="A52" s="82"/>
       <c r="B52" s="10" t="s">
         <v>63</v>
       </c>
@@ -2581,7 +2587,7 @@
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A53" s="74"/>
+      <c r="A53" s="82"/>
       <c r="B53" s="10" t="s">
         <v>68</v>
       </c>
@@ -2591,7 +2597,7 @@
       <c r="D53" s="21"/>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A54" s="74"/>
+      <c r="A54" s="82"/>
       <c r="B54" s="10" t="s">
         <v>70</v>
       </c>
@@ -2601,7 +2607,7 @@
       <c r="D54" s="21"/>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A55" s="74"/>
+      <c r="A55" s="82"/>
       <c r="B55" s="10" t="s">
         <v>72</v>
       </c>
@@ -2611,7 +2617,7 @@
       <c r="D55" s="21"/>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A56" s="74"/>
+      <c r="A56" s="82"/>
       <c r="B56" s="10" t="s">
         <v>49</v>
       </c>
@@ -2621,7 +2627,7 @@
       <c r="D56" s="21"/>
     </row>
     <row r="57" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="75"/>
+      <c r="A57" s="83"/>
       <c r="B57" s="12" t="s">
         <v>73</v>
       </c>
@@ -2631,7 +2637,7 @@
       <c r="D57" s="23"/>
     </row>
     <row r="58" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A58" s="73" t="s">
+      <c r="A58" s="81" t="s">
         <v>74</v>
       </c>
       <c r="B58" s="8" t="s">
@@ -2645,7 +2651,7 @@
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" s="74"/>
+      <c r="A59" s="82"/>
       <c r="B59" s="10" t="s">
         <v>76</v>
       </c>
@@ -2657,7 +2663,7 @@
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A60" s="74"/>
+      <c r="A60" s="82"/>
       <c r="B60" s="10" t="s">
         <v>79</v>
       </c>
@@ -2669,7 +2675,7 @@
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A61" s="74"/>
+      <c r="A61" s="82"/>
       <c r="B61" s="10" t="s">
         <v>81</v>
       </c>
@@ -2681,7 +2687,7 @@
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A62" s="74"/>
+      <c r="A62" s="82"/>
       <c r="B62" s="10" t="s">
         <v>82</v>
       </c>
@@ -2693,7 +2699,7 @@
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A63" s="74"/>
+      <c r="A63" s="82"/>
       <c r="B63" s="10" t="s">
         <v>85</v>
       </c>
@@ -2705,7 +2711,7 @@
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="74"/>
+      <c r="A64" s="82"/>
       <c r="B64" s="10" t="s">
         <v>86</v>
       </c>
@@ -2717,7 +2723,7 @@
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" s="74"/>
+      <c r="A65" s="82"/>
       <c r="B65" s="10" t="s">
         <v>88</v>
       </c>
@@ -2729,7 +2735,7 @@
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" s="74"/>
+      <c r="A66" s="82"/>
       <c r="B66" s="10" t="s">
         <v>90</v>
       </c>
@@ -2741,7 +2747,7 @@
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A67" s="74"/>
+      <c r="A67" s="82"/>
       <c r="B67" s="10" t="s">
         <v>92</v>
       </c>
@@ -2753,7 +2759,7 @@
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A68" s="74"/>
+      <c r="A68" s="82"/>
       <c r="B68" s="10" t="s">
         <v>94</v>
       </c>
@@ -2765,7 +2771,7 @@
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A69" s="74"/>
+      <c r="A69" s="82"/>
       <c r="B69" s="10" t="s">
         <v>96</v>
       </c>
@@ -2777,7 +2783,7 @@
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A70" s="74"/>
+      <c r="A70" s="82"/>
       <c r="B70" s="10" t="s">
         <v>98</v>
       </c>
@@ -2789,7 +2795,7 @@
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A71" s="74"/>
+      <c r="A71" s="82"/>
       <c r="B71" s="10" t="s">
         <v>100</v>
       </c>
@@ -2801,7 +2807,7 @@
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A72" s="74"/>
+      <c r="A72" s="82"/>
       <c r="B72" s="10" t="s">
         <v>102</v>
       </c>
@@ -2813,7 +2819,7 @@
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A73" s="74"/>
+      <c r="A73" s="82"/>
       <c r="B73" s="10" t="s">
         <v>105</v>
       </c>
@@ -2825,7 +2831,7 @@
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A74" s="74"/>
+      <c r="A74" s="82"/>
       <c r="B74" s="10" t="s">
         <v>106</v>
       </c>
@@ -2837,7 +2843,7 @@
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="74"/>
+      <c r="A75" s="82"/>
       <c r="B75" s="10" t="s">
         <v>108</v>
       </c>
@@ -2849,7 +2855,7 @@
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" s="74"/>
+      <c r="A76" s="82"/>
       <c r="B76" s="10" t="s">
         <v>109</v>
       </c>
@@ -2861,7 +2867,7 @@
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" s="74"/>
+      <c r="A77" s="82"/>
       <c r="B77" s="10" t="s">
         <v>110</v>
       </c>
@@ -2873,7 +2879,7 @@
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A78" s="74"/>
+      <c r="A78" s="82"/>
       <c r="B78" s="10" t="s">
         <v>111</v>
       </c>
@@ -2885,7 +2891,7 @@
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A79" s="74"/>
+      <c r="A79" s="82"/>
       <c r="B79" s="10" t="s">
         <v>112</v>
       </c>
@@ -2897,7 +2903,7 @@
       </c>
     </row>
     <row r="80" spans="1:4" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A80" s="75"/>
+      <c r="A80" s="83"/>
       <c r="B80" s="12" t="s">
         <v>49</v>
       </c>
@@ -2909,7 +2915,7 @@
       </c>
     </row>
     <row r="81" spans="1:4" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A81" s="73" t="s">
+      <c r="A81" s="81" t="s">
         <v>114</v>
       </c>
       <c r="B81" s="8" t="s">
@@ -2923,7 +2929,7 @@
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="74"/>
+      <c r="A82" s="82"/>
       <c r="B82" s="10" t="s">
         <v>116</v>
       </c>
@@ -2935,7 +2941,7 @@
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" s="74"/>
+      <c r="A83" s="82"/>
       <c r="B83" s="10" t="s">
         <v>117</v>
       </c>
@@ -2947,7 +2953,7 @@
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" s="74"/>
+      <c r="A84" s="82"/>
       <c r="B84" s="10" t="s">
         <v>118</v>
       </c>
@@ -2959,7 +2965,7 @@
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A85" s="74"/>
+      <c r="A85" s="82"/>
       <c r="B85" s="10" t="s">
         <v>119</v>
       </c>
@@ -2971,7 +2977,7 @@
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A86" s="74"/>
+      <c r="A86" s="82"/>
       <c r="B86" s="10" t="s">
         <v>120</v>
       </c>
@@ -2983,7 +2989,7 @@
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A87" s="74"/>
+      <c r="A87" s="82"/>
       <c r="B87" s="10" t="s">
         <v>121</v>
       </c>
@@ -2995,7 +3001,7 @@
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A88" s="74"/>
+      <c r="A88" s="82"/>
       <c r="B88" s="10" t="s">
         <v>122</v>
       </c>
@@ -3007,7 +3013,7 @@
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A89" s="74"/>
+      <c r="A89" s="82"/>
       <c r="B89" s="10" t="s">
         <v>123</v>
       </c>
@@ -3019,7 +3025,7 @@
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="74"/>
+      <c r="A90" s="82"/>
       <c r="B90" s="10" t="s">
         <v>124</v>
       </c>
@@ -3031,7 +3037,7 @@
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" s="74"/>
+      <c r="A91" s="82"/>
       <c r="B91" s="10" t="s">
         <v>125</v>
       </c>
@@ -3043,7 +3049,7 @@
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" s="74"/>
+      <c r="A92" s="82"/>
       <c r="B92" s="10" t="s">
         <v>126</v>
       </c>
@@ -3055,7 +3061,7 @@
       </c>
     </row>
     <row r="93" spans="1:4" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A93" s="75"/>
+      <c r="A93" s="83"/>
       <c r="B93" s="12" t="s">
         <v>49</v>
       </c>
@@ -6540,17 +6546,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{99807E8C-EE63-4A76-8E1C-D22B4AB455E8}">
   <dimension ref="A1:R18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="60" zoomScaleNormal="60" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5:E5"/>
+    <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="37.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="60.7109375" style="1" customWidth="1"/>
+    <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
+    <col min="3" max="3" width="74.28515625" style="1" customWidth="1"/>
     <col min="4" max="5" width="40.7109375" style="1" customWidth="1"/>
-    <col min="6" max="12" width="9.140625" style="1"/>
+    <col min="6" max="9" width="9.140625" style="1"/>
+    <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="9.140625" style="1"/>
     <col min="13" max="13" width="12.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="14" max="17" width="9.140625" style="1"/>
     <col min="18" max="18" width="11.140625" style="1" bestFit="1" customWidth="1"/>
@@ -6558,237 +6566,238 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:18" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="89" t="s">
+      <c r="A1" s="99" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="89"/>
-      <c r="C1" s="89"/>
-      <c r="D1" s="89"/>
-      <c r="E1" s="89"/>
+      <c r="B1" s="99"/>
+      <c r="C1" s="99"/>
+      <c r="D1" s="99"/>
+      <c r="E1" s="99"/>
     </row>
     <row r="2" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="100" t="s">
         <v>263</v>
       </c>
       <c r="B2" s="93"/>
-      <c r="C2" s="79">
+      <c r="C2" s="50">
         <v>10</v>
       </c>
-      <c r="D2" s="84" t="s">
+      <c r="D2" s="48" t="s">
         <v>242</v>
       </c>
-      <c r="E2" s="80">
+      <c r="E2" s="51">
         <v>17000</v>
       </c>
     </row>
     <row r="3" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="92" t="s">
+      <c r="A3" s="91" t="s">
         <v>253</v>
       </c>
       <c r="B3" s="93"/>
-      <c r="C3" s="79">
+      <c r="C3" s="50">
         <f>C2*5</f>
         <v>50</v>
       </c>
-      <c r="D3" s="84" t="s">
+      <c r="D3" s="48" t="s">
         <v>254</v>
       </c>
-      <c r="E3" s="80">
+      <c r="E3" s="51">
         <f>C3*E2</f>
         <v>850000</v>
       </c>
     </row>
     <row r="4" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="92" t="s">
+      <c r="A4" s="91" t="s">
         <v>255</v>
       </c>
       <c r="B4" s="93"/>
-      <c r="C4" s="79">
+      <c r="C4" s="50">
         <f>SUM(D7:D14)</f>
         <v>12</v>
       </c>
-      <c r="D4" s="84" t="s">
+      <c r="D4" s="48" t="s">
         <v>256</v>
       </c>
-      <c r="E4" s="95">
-        <f>(E3*C4)-((E3*C4)*0%)</f>
-        <v>10200000</v>
-      </c>
+      <c r="E4" s="55">
+        <f>(E3*C4)-((E3*C4)*6.86275%)</f>
+        <v>9499999.5</v>
+      </c>
+      <c r="J4" s="43"/>
     </row>
     <row r="5" spans="1:18" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="81"/>
-      <c r="B5" s="82"/>
-      <c r="C5" s="82"/>
-      <c r="D5" s="82"/>
-      <c r="E5" s="83"/>
+      <c r="A5" s="88"/>
+      <c r="B5" s="89"/>
+      <c r="C5" s="89"/>
+      <c r="D5" s="89"/>
+      <c r="E5" s="90"/>
       <c r="R5" s="43"/>
     </row>
     <row r="6" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A6" s="87" t="s">
+      <c r="A6" s="52" t="s">
         <v>261</v>
       </c>
-      <c r="B6" s="84" t="s">
+      <c r="B6" s="48" t="s">
         <v>251</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="D6" s="84" t="s">
+      <c r="D6" s="48" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="84" t="s">
+      <c r="E6" s="48" t="s">
         <v>252</v>
       </c>
       <c r="M6" s="43"/>
     </row>
     <row r="7" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="77">
+      <c r="A7" s="94">
         <v>1</v>
       </c>
-      <c r="B7" s="77" t="s">
+      <c r="B7" s="94" t="s">
         <v>234</v>
       </c>
-      <c r="C7" s="84" t="s">
+      <c r="C7" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="85">
+      <c r="D7" s="95">
         <v>2</v>
       </c>
-      <c r="E7" s="86">
+      <c r="E7" s="96">
         <f>$E$4*5%</f>
-        <v>510000</v>
+        <v>474999.97500000003</v>
       </c>
     </row>
     <row r="8" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="77"/>
-      <c r="B8" s="77"/>
-      <c r="C8" s="87" t="s">
+      <c r="A8" s="94"/>
+      <c r="B8" s="94"/>
+      <c r="C8" s="52" t="s">
         <v>259</v>
       </c>
-      <c r="D8" s="85"/>
-      <c r="E8" s="85"/>
+      <c r="D8" s="95"/>
+      <c r="E8" s="95"/>
     </row>
     <row r="9" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="90">
+      <c r="A9" s="54">
         <v>2</v>
       </c>
-      <c r="B9" s="90" t="s">
+      <c r="B9" s="97" t="s">
         <v>236</v>
       </c>
-      <c r="C9" s="91"/>
-      <c r="D9" s="88">
+      <c r="C9" s="98"/>
+      <c r="D9" s="53">
         <v>2</v>
       </c>
-      <c r="E9" s="80">
+      <c r="E9" s="51">
         <f>$E$4*10%</f>
-        <v>1020000</v>
+        <v>949999.95000000007</v>
       </c>
     </row>
     <row r="10" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="84">
+      <c r="A10" s="48">
         <v>3</v>
       </c>
-      <c r="B10" s="84" t="s">
+      <c r="B10" s="91" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="78"/>
-      <c r="D10" s="79">
+      <c r="C10" s="93"/>
+      <c r="D10" s="50">
         <v>1</v>
       </c>
-      <c r="E10" s="80">
+      <c r="E10" s="51">
         <f>$E$4*10%</f>
-        <v>1020000</v>
+        <v>949999.95000000007</v>
       </c>
     </row>
     <row r="11" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="77">
+      <c r="A11" s="94">
         <v>4</v>
       </c>
-      <c r="B11" s="77" t="s">
+      <c r="B11" s="94" t="s">
         <v>1</v>
       </c>
-      <c r="C11" s="84" t="s">
+      <c r="C11" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D11" s="79">
+      <c r="D11" s="50">
         <v>1</v>
       </c>
-      <c r="E11" s="86">
+      <c r="E11" s="96">
         <f>$E$4*60%</f>
-        <v>6120000</v>
+        <v>5699999.7000000002</v>
       </c>
     </row>
     <row r="12" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="77"/>
-      <c r="B12" s="77"/>
-      <c r="C12" s="84" t="s">
-        <v>231</v>
-      </c>
-      <c r="D12" s="79">
+      <c r="A12" s="94"/>
+      <c r="B12" s="94"/>
+      <c r="C12" s="48" t="s">
+        <v>265</v>
+      </c>
+      <c r="D12" s="50">
         <v>3</v>
       </c>
-      <c r="E12" s="85"/>
+      <c r="E12" s="95"/>
     </row>
     <row r="13" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="77">
+      <c r="A13" s="94">
         <v>5</v>
       </c>
-      <c r="B13" s="77" t="s">
+      <c r="B13" s="94" t="s">
         <v>238</v>
       </c>
-      <c r="C13" s="78" t="s">
+      <c r="C13" s="49" t="s">
         <v>239</v>
       </c>
-      <c r="D13" s="79">
+      <c r="D13" s="50">
         <v>1.5</v>
       </c>
-      <c r="E13" s="80">
+      <c r="E13" s="51">
         <f>$E$4*7.5%</f>
-        <v>765000</v>
+        <v>712499.96250000002</v>
       </c>
     </row>
     <row r="14" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="77"/>
-      <c r="B14" s="77"/>
-      <c r="C14" s="78" t="s">
+      <c r="A14" s="94"/>
+      <c r="B14" s="94"/>
+      <c r="C14" s="49" t="s">
         <v>240</v>
       </c>
-      <c r="D14" s="79">
+      <c r="D14" s="50">
         <v>1.5</v>
       </c>
-      <c r="E14" s="80">
+      <c r="E14" s="51">
         <f>$E$4*7.5%</f>
-        <v>765000</v>
+        <v>712499.96250000002</v>
       </c>
     </row>
     <row r="15" spans="1:18" ht="39.950000000000003" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="81"/>
-      <c r="B15" s="82"/>
-      <c r="C15" s="82"/>
-      <c r="D15" s="82"/>
-      <c r="E15" s="83"/>
+      <c r="A15" s="88"/>
+      <c r="B15" s="89"/>
+      <c r="C15" s="89"/>
+      <c r="D15" s="89"/>
+      <c r="E15" s="90"/>
     </row>
     <row r="16" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="92" t="s">
+      <c r="A16" s="91" t="s">
         <v>262</v>
       </c>
-      <c r="B16" s="99"/>
-      <c r="C16" s="99"/>
-      <c r="D16" s="99"/>
+      <c r="B16" s="92"/>
+      <c r="C16" s="92"/>
+      <c r="D16" s="92"/>
       <c r="E16" s="93"/>
     </row>
     <row r="17" spans="1:5" ht="300" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="96" t="s">
+      <c r="A17" s="85" t="s">
         <v>264</v>
       </c>
-      <c r="B17" s="97"/>
-      <c r="C17" s="97"/>
-      <c r="D17" s="97"/>
-      <c r="E17" s="98"/>
+      <c r="B17" s="86"/>
+      <c r="C17" s="86"/>
+      <c r="D17" s="86"/>
+      <c r="E17" s="87"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
-  <mergeCells count="17">
+  <mergeCells count="19">
     <mergeCell ref="A1:E1"/>
     <mergeCell ref="B7:B8"/>
     <mergeCell ref="B11:B12"/>
@@ -6796,6 +6805,7 @@
     <mergeCell ref="A2:B2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
+    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A15:E15"/>
@@ -6806,6 +6816,7 @@
     <mergeCell ref="A11:A12"/>
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A13:A14"/>
+    <mergeCell ref="B9:C9"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.11811023622047245" footer="0.11811023622047245"/>

</xml_diff>

<commit_message>
implementacion del modulo de creacion y validacion de empresas existentes
</commit_message>
<xml_diff>
--- a/public/recursos/Cotizacion-modulos.xlsx
+++ b/public/recursos/Cotizacion-modulos.xlsx
@@ -8,17 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\WWW\avaluamos\public\recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36C1B0BF-C92F-4E3D-83FF-AFA151831BB1}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7D02F07-15DF-41E7-8E8C-DA83CE37B17F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Diseño" sheetId="1" r:id="rId1"/>
+    <sheet name="Borrador" sheetId="1" r:id="rId1"/>
     <sheet name="Avalúo" sheetId="2" r:id="rId2"/>
     <sheet name="Dptos" sheetId="3" r:id="rId3"/>
     <sheet name="Ciudades" sheetId="4" r:id="rId4"/>
     <sheet name="Paises" sheetId="5" r:id="rId5"/>
-    <sheet name="Diseño (2)" sheetId="6" r:id="rId6"/>
+    <sheet name="Cotización" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -917,7 +917,7 @@
     </font>
     <font>
       <b/>
-      <sz val="20"/>
+      <sz val="24"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -925,7 +925,7 @@
     </font>
     <font>
       <b/>
-      <sz val="24"/>
+      <sz val="48"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -1000,7 +1000,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="20">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -1216,42 +1216,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top/>
-      <bottom style="double">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="101">
+  <cellXfs count="106">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1415,7 +1384,7 @@
     <xf numFmtId="0" fontId="7" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="8" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1505,14 +1474,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1523,35 +1492,50 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="6" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1" shrinkToFit="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="6" fillId="10" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="11" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="10" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -6547,7 +6531,7 @@
   <dimension ref="A1:R18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+      <selection sqref="A1:E1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6555,7 +6539,7 @@
     <col min="1" max="1" width="25.140625" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="55.7109375" style="1" customWidth="1"/>
     <col min="3" max="3" width="74.28515625" style="1" customWidth="1"/>
-    <col min="4" max="5" width="40.7109375" style="1" customWidth="1"/>
+    <col min="4" max="5" width="45.7109375" style="1" customWidth="1"/>
     <col min="6" max="9" width="9.140625" style="1"/>
     <col min="10" max="10" width="12.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="12" width="9.140625" style="1"/>
@@ -6565,20 +6549,20 @@
     <col min="19" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="50.1" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="99" t="s">
+    <row r="1" spans="1:18" ht="99.95" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="103" t="s">
         <v>260</v>
       </c>
-      <c r="B1" s="99"/>
-      <c r="C1" s="99"/>
-      <c r="D1" s="99"/>
-      <c r="E1" s="99"/>
-    </row>
-    <row r="2" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="100" t="s">
+      <c r="B1" s="104"/>
+      <c r="C1" s="104"/>
+      <c r="D1" s="104"/>
+      <c r="E1" s="105"/>
+    </row>
+    <row r="2" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="85" t="s">
         <v>263</v>
       </c>
-      <c r="B2" s="93"/>
+      <c r="B2" s="86"/>
       <c r="C2" s="50">
         <v>10</v>
       </c>
@@ -6589,11 +6573,11 @@
         <v>17000</v>
       </c>
     </row>
-    <row r="3" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="91" t="s">
+    <row r="3" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="87" t="s">
         <v>253</v>
       </c>
-      <c r="B3" s="93"/>
+      <c r="B3" s="86"/>
       <c r="C3" s="50">
         <f>C2*5</f>
         <v>50</v>
@@ -6606,11 +6590,11 @@
         <v>850000</v>
       </c>
     </row>
-    <row r="4" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="91" t="s">
+    <row r="4" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="87" t="s">
         <v>255</v>
       </c>
-      <c r="B4" s="93"/>
+      <c r="B4" s="86"/>
       <c r="C4" s="50">
         <f>SUM(D7:D14)</f>
         <v>12</v>
@@ -6632,7 +6616,7 @@
       <c r="E5" s="90"/>
       <c r="R5" s="43"/>
     </row>
-    <row r="6" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="52" t="s">
         <v>261</v>
       </c>
@@ -6642,49 +6626,49 @@
       <c r="C6" s="48" t="s">
         <v>258</v>
       </c>
-      <c r="D6" s="48" t="s">
+      <c r="D6" s="94" t="s">
         <v>257</v>
       </c>
-      <c r="E6" s="48" t="s">
+      <c r="E6" s="94" t="s">
         <v>252</v>
       </c>
       <c r="M6" s="43"/>
     </row>
-    <row r="7" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="94">
+    <row r="7" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="95">
         <v>1</v>
       </c>
-      <c r="B7" s="94" t="s">
+      <c r="B7" s="95" t="s">
         <v>234</v>
       </c>
       <c r="C7" s="48" t="s">
         <v>243</v>
       </c>
-      <c r="D7" s="95">
+      <c r="D7" s="99">
         <v>2</v>
       </c>
-      <c r="E7" s="96">
+      <c r="E7" s="97">
         <f>$E$4*5%</f>
         <v>474999.97500000003</v>
       </c>
     </row>
-    <row r="8" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A8" s="94"/>
-      <c r="B8" s="94"/>
+    <row r="8" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="96"/>
+      <c r="B8" s="96"/>
       <c r="C8" s="52" t="s">
         <v>259</v>
       </c>
-      <c r="D8" s="95"/>
-      <c r="E8" s="95"/>
-    </row>
-    <row r="9" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D8" s="98"/>
+      <c r="E8" s="98"/>
+    </row>
+    <row r="9" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="54">
         <v>2</v>
       </c>
-      <c r="B9" s="97" t="s">
+      <c r="B9" s="92" t="s">
         <v>236</v>
       </c>
-      <c r="C9" s="98"/>
+      <c r="C9" s="93"/>
       <c r="D9" s="53">
         <v>2</v>
       </c>
@@ -6693,14 +6677,14 @@
         <v>949999.95000000007</v>
       </c>
     </row>
-    <row r="10" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="48">
         <v>3</v>
       </c>
-      <c r="B10" s="91" t="s">
+      <c r="B10" s="87" t="s">
         <v>232</v>
       </c>
-      <c r="C10" s="93"/>
+      <c r="C10" s="86"/>
       <c r="D10" s="50">
         <v>1</v>
       </c>
@@ -6709,11 +6693,11 @@
         <v>949999.95000000007</v>
       </c>
     </row>
-    <row r="11" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="94">
+    <row r="11" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="95">
         <v>4</v>
       </c>
-      <c r="B11" s="94" t="s">
+      <c r="B11" s="95" t="s">
         <v>1</v>
       </c>
       <c r="C11" s="48" t="s">
@@ -6722,27 +6706,27 @@
       <c r="D11" s="50">
         <v>1</v>
       </c>
-      <c r="E11" s="96">
+      <c r="E11" s="97">
         <f>$E$4*60%</f>
         <v>5699999.7000000002</v>
       </c>
     </row>
-    <row r="12" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A12" s="94"/>
-      <c r="B12" s="94"/>
+    <row r="12" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A12" s="96"/>
+      <c r="B12" s="96"/>
       <c r="C12" s="48" t="s">
         <v>265</v>
       </c>
       <c r="D12" s="50">
         <v>3</v>
       </c>
-      <c r="E12" s="95"/>
-    </row>
-    <row r="13" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="94">
+      <c r="E12" s="98"/>
+    </row>
+    <row r="13" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="95">
         <v>5</v>
       </c>
-      <c r="B13" s="94" t="s">
+      <c r="B13" s="95" t="s">
         <v>238</v>
       </c>
       <c r="C13" s="49" t="s">
@@ -6756,9 +6740,9 @@
         <v>712499.96250000002</v>
       </c>
     </row>
-    <row r="14" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="94"/>
-      <c r="B14" s="94"/>
+    <row r="14" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="96"/>
+      <c r="B14" s="96"/>
       <c r="C14" s="49" t="s">
         <v>240</v>
       </c>
@@ -6777,35 +6761,27 @@
       <c r="D15" s="89"/>
       <c r="E15" s="90"/>
     </row>
-    <row r="16" spans="1:18" ht="60" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="91" t="s">
+    <row r="16" spans="1:18" ht="80.099999999999994" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="87" t="s">
         <v>262</v>
       </c>
-      <c r="B16" s="92"/>
-      <c r="C16" s="92"/>
-      <c r="D16" s="92"/>
-      <c r="E16" s="93"/>
+      <c r="B16" s="91"/>
+      <c r="C16" s="91"/>
+      <c r="D16" s="91"/>
+      <c r="E16" s="86"/>
     </row>
     <row r="17" spans="1:5" ht="300" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="85" t="s">
+      <c r="A17" s="100" t="s">
         <v>264</v>
       </c>
-      <c r="B17" s="86"/>
-      <c r="C17" s="86"/>
-      <c r="D17" s="86"/>
-      <c r="E17" s="87"/>
+      <c r="B17" s="101"/>
+      <c r="C17" s="101"/>
+      <c r="D17" s="101"/>
+      <c r="E17" s="102"/>
     </row>
     <row r="18" spans="1:5" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="19">
-    <mergeCell ref="A1:E1"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="B11:B12"/>
-    <mergeCell ref="B13:B14"/>
-    <mergeCell ref="A2:B2"/>
-    <mergeCell ref="A3:B3"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="B10:C10"/>
     <mergeCell ref="A17:E17"/>
     <mergeCell ref="A5:E5"/>
     <mergeCell ref="A15:E15"/>
@@ -6817,9 +6793,17 @@
     <mergeCell ref="E11:E12"/>
     <mergeCell ref="A13:A14"/>
     <mergeCell ref="B9:C9"/>
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="B13:B14"/>
+    <mergeCell ref="A2:B2"/>
+    <mergeCell ref="A3:B3"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="B10:C10"/>
   </mergeCells>
   <printOptions horizontalCentered="1"/>
-  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0.11811023622047245" footer="0.11811023622047245"/>
-  <pageSetup scale="50" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageMargins left="0.39370078740157483" right="0.39370078740157483" top="0.39370078740157483" bottom="0.39370078740157483" header="0" footer="0"/>
+  <pageSetup scale="40" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>